<commit_message>
cleared values in test sheet
</commit_message>
<xml_diff>
--- a/xlwings/tests/test1.xlsx
+++ b/xlwings/tests/test1.xlsx
@@ -26,17 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="3">
-  <si>
-    <t>éöà</t>
-  </si>
-  <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -375,114 +365,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A2:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2.222</v>
-      </c>
-      <c r="E1">
-        <v>3.3</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>2.222</v>
-      </c>
-      <c r="J1">
-        <v>3.3</v>
-      </c>
-      <c r="L1">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="M1">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="N1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>22953</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="M2">
-        <v>5.5</v>
-      </c>
-      <c r="N2">
-        <v>6.6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="C3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="E3">
-        <v>9.9990000000000006</v>
-      </c>
-      <c r="H3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="J3">
-        <v>9.9990000000000006</v>
-      </c>
-      <c r="L3">
-        <v>7.7</v>
-      </c>
-      <c r="M3">
-        <v>8.8000000000000007</v>
-      </c>
-      <c r="N3">
-        <v>65535</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>22.222000000000001</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -491,87 +388,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A2:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2.222</v>
-      </c>
-      <c r="E1">
-        <v>3.3</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>2.222</v>
-      </c>
-      <c r="J1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>22953</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="C3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="E3">
-        <v>9.9990000000000006</v>
-      </c>
-      <c r="H3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="J3">
-        <v>9.9990000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>22.222000000000001</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -580,87 +411,21 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A2:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:J3"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2.222</v>
-      </c>
-      <c r="E1">
-        <v>3.3</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-      <c r="I1">
-        <v>2.222</v>
-      </c>
-      <c r="J1">
-        <v>3.3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>22953</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="C3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="D3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="E3">
-        <v>9.9990000000000006</v>
-      </c>
-      <c r="H3" s="1">
-        <v>22953</v>
-      </c>
-      <c r="I3" s="2">
-        <v>44196.508564814816</v>
-      </c>
-      <c r="J3">
-        <v>9.9990000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>22.222000000000001</v>
-      </c>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="2"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fix and additional tests for None handling if atleast_2d=True
</commit_message>
<xml_diff>
--- a/xlwings/tests/test1.xlsx
+++ b/xlwings/tests/test1.xlsx
@@ -12,6 +12,11 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet7" sheetId="7" r:id="rId7"/>
+    <sheet name="Sheet8" sheetId="8" r:id="rId8"/>
+    <sheet name="Sheet9" sheetId="9" r:id="rId9"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="cell_sheet1">Sheet1!$A$14</definedName>
@@ -23,10 +28,6 @@
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,6 +387,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I3"/>
@@ -454,4 +467,52 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>